<commit_message>
Added final presentation slides
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yeelongsiah/Desktop/School/NTU/SC2001/Dijkstra's Alg/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F9A08DA-4963-4848-AD69-35143FEA9EC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA115A06-AC47-D047-8E80-31445D376063}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{8A83C292-6E76-F249-AC67-58BE18C7F3DB}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{8A83C292-6E76-F249-AC67-58BE18C7F3DB}"/>
   </bookViews>
   <sheets>
     <sheet name="results" sheetId="1" r:id="rId1"/>
@@ -85,7 +85,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -138,8 +138,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -147,11 +147,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1908,6 +1908,655 @@
 </file>
 
 <file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="960" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>60% connected graph</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="960" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>list</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>results!$A$3:$A$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1400</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1600</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1800</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2200</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2400</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2600</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2800</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3200</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3400</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3600</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3800</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>results!$G$3:$G$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>4.4140000000000004E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.6830000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.1789999999999996E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.1169E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.7786E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.7015000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.7541999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.9732999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.3573000000000005E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7.9016000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9.8225000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.121863</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.15376699999999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.16777600000000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.19556299999999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.25959900000000002</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.25430399999999997</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.29503099999999999</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.36471700000000001</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.36584</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-355C-644F-B5F7-5B9A0A0D0DF7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>theoretical list</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>results!$W$3:$W$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>4.5633821452955098E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.1386783436641385E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.492576846813899E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.6986117259024021E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.466863875283068E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.3245501898696924E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.1493229187816539E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.2677490011103587E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.7273201442088658E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.5761808355118523E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8.8630551503233859E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.11637188368631836</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.14948299307789317</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.18846540662386987</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.23382465486320933</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.28606998490436619</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.34571411186055784</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.41327300148988788</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.48926567850474051</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.57421405625236421</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-355C-644F-B5F7-5B9A0A0D0DF7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="192770208"/>
+        <c:axId val="192766768"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="192770208"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>size</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> V</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="192766768"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="192766768"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>runtime</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="192770208"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="800"/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-GB"/>
@@ -3192,9 +3841,8 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="1"/>
@@ -3203,15 +3851,17 @@
             <c:v>matrix</c:v>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
           <c:cat>
             <c:numRef>
               <c:f>results!$A$3:$A$22</c:f>
@@ -3350,6 +4000,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-9E50-D045-BD81-3F21B4EDAE95}"/>
@@ -3357,162 +4008,96 @@
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="2"/>
+          <c:idx val="0"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>list</c:v>
+            <c:v>theoretical matrix</c:v>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
             <c:numRef>
-              <c:f>results!$A$3:$A$22</c:f>
+              <c:f>results!$V$3:$V$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>200</c:v>
+                  <c:v>3.48E-4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>400</c:v>
+                  <c:v>1.392E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>600</c:v>
+                  <c:v>3.1320000000000002E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>800</c:v>
+                  <c:v>5.568E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1000</c:v>
+                  <c:v>8.6999999999999994E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1200</c:v>
+                  <c:v>1.2528000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1400</c:v>
+                  <c:v>1.7052000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1600</c:v>
+                  <c:v>2.2272E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1800</c:v>
+                  <c:v>2.8188000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2000</c:v>
+                  <c:v>3.4799999999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2200</c:v>
+                  <c:v>4.2108E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2400</c:v>
+                  <c:v>5.0112000000000004E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2600</c:v>
+                  <c:v>5.8812000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2800</c:v>
+                  <c:v>6.8208000000000005E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3000</c:v>
+                  <c:v>7.8299999999999995E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3200</c:v>
+                  <c:v>8.9088000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3400</c:v>
+                  <c:v>0.10057200000000001</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>3600</c:v>
+                  <c:v>0.112752</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>3800</c:v>
+                  <c:v>0.12562799999999999</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>4000</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>results!$G$3:$G$22</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
-                <c:pt idx="0">
-                  <c:v>4.4140000000000004E-3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.6830000000000001E-3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>6.1789999999999996E-3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.1169E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.7786E-2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2.7015000000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3.7541999999999999E-2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>4.9732999999999999E-2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>6.3573000000000005E-2</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>7.9016000000000003E-2</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>9.8225000000000007E-2</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.121863</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.15376699999999999</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.16777600000000001</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.19556299999999999</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.25959900000000002</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.25430399999999997</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.29503099999999999</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.36471700000000001</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0.36584</c:v>
+                  <c:v>0.13919999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-9E50-D045-BD81-3F21B4EDAE95}"/>
+              <c16:uniqueId val="{00000000-A3DC-AF47-9400-80DD168FA73C}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3524,10 +4109,10 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="150"/>
+        <c:smooth val="0"/>
         <c:axId val="192770208"/>
         <c:axId val="192766768"/>
-      </c:barChart>
+      </c:lineChart>
       <c:catAx>
         <c:axId val="192770208"/>
         <c:scaling>
@@ -3535,6 +4120,66 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>size</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> V</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3600,6 +4245,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>runtime</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -8613,6 +9313,46 @@
 </file>
 
 <file path=xl/charts/colors11.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors12.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -10005,6 +10745,522 @@
 </file>
 
 <file path=xl/charts/style11.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style12.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -14700,16 +15956,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>279400</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>2715099</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>159723</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>2641601</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>138543</xdr:rowOff>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>1707931</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>153277</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -15038,6 +16294,44 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>2484175</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>181429</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>1477008</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>174983</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="13" name="Chart 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B17D384E-DFE5-BD47-9FBE-433C592ADF98}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId12"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -15379,13 +16673,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C20B9EC-4AA2-AE46-8826-2B4D3F091796}">
-  <dimension ref="A1:W117"/>
+  <dimension ref="A1:Y117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="44" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+    <sheetView tabSelected="1" topLeftCell="S2" zoomScale="50" zoomScaleNormal="198" workbookViewId="0">
+      <selection activeCell="Z21" sqref="Z21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="47"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="47" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="43.83203125" style="1" bestFit="1" customWidth="1"/>
@@ -15397,13 +16691,13 @@
     <col min="8" max="8" width="43.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="34.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="43.83203125" style="1" customWidth="1"/>
-    <col min="12" max="18" width="43.83203125" style="7" customWidth="1"/>
+    <col min="12" max="18" width="43.83203125" style="3" customWidth="1"/>
     <col min="19" max="19" width="43.83203125" customWidth="1"/>
     <col min="20" max="32" width="43.83203125" style="1" customWidth="1"/>
     <col min="33" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" s="4">
         <v>1</v>
       </c>
@@ -15447,7 +16741,7 @@
       <c r="V1" s="4"/>
       <c r="W1" s="5"/>
     </row>
-    <row r="2" spans="1:23">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -15508,8 +16802,14 @@
       <c r="U2" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="X2" s="1">
+        <v>8.7000000000000001E-9</v>
+      </c>
+      <c r="Y2" s="1">
+        <v>4.9999999999999997E-12</v>
+      </c>
     </row>
-    <row r="3" spans="1:23">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1">
         <v>200</v>
       </c>
@@ -15573,8 +16873,16 @@
       <c r="U3" s="1">
         <v>1.2110000000000001E-3</v>
       </c>
+      <c r="V3" s="1">
+        <f>A3*A3*$X$2</f>
+        <v>3.48E-4</v>
+      </c>
+      <c r="W3" s="1">
+        <f>(A3*((A3*(A3-1))/2)*0.3)*LOG(A3,2)*$Y$2</f>
+        <v>4.5633821452955098E-5</v>
+      </c>
     </row>
-    <row r="4" spans="1:23">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1">
         <f>A3+200</f>
         <v>400</v>
@@ -15639,10 +16947,18 @@
       <c r="U4" s="1">
         <v>3.77E-4</v>
       </c>
+      <c r="V4" s="1">
+        <f t="shared" ref="V4:V22" si="0">A4*A4*$X$2</f>
+        <v>1.392E-3</v>
+      </c>
+      <c r="W4" s="1">
+        <f t="shared" ref="W4:W22" si="1">(A4*((A4*(A4-1))/2)*0.3)*LOG(A4,2)*$Y$2</f>
+        <v>4.1386783436641385E-4</v>
+      </c>
     </row>
-    <row r="5" spans="1:23">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1">
-        <f t="shared" ref="A5:A39" si="0">A4+200</f>
+        <f t="shared" ref="A5:A22" si="2">A4+200</f>
         <v>600</v>
       </c>
       <c r="B5" s="1">
@@ -15705,10 +17021,18 @@
       <c r="U5" s="1">
         <v>9.0499999999999999E-4</v>
       </c>
+      <c r="V5" s="1">
+        <f t="shared" si="0"/>
+        <v>3.1320000000000002E-3</v>
+      </c>
+      <c r="W5" s="1">
+        <f t="shared" si="1"/>
+        <v>1.492576846813899E-3</v>
+      </c>
     </row>
-    <row r="6" spans="1:23">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>800</v>
       </c>
       <c r="B6" s="1">
@@ -15771,10 +17095,18 @@
       <c r="U6" s="1">
         <v>1.8220000000000001E-3</v>
       </c>
+      <c r="V6" s="1">
+        <f t="shared" si="0"/>
+        <v>5.568E-3</v>
+      </c>
+      <c r="W6" s="1">
+        <f t="shared" si="1"/>
+        <v>3.6986117259024021E-3</v>
+      </c>
     </row>
-    <row r="7" spans="1:23">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1000</v>
       </c>
       <c r="B7" s="1">
@@ -15837,10 +17169,18 @@
       <c r="U7" s="1">
         <v>2.9759999999999999E-3</v>
       </c>
+      <c r="V7" s="1">
+        <f t="shared" si="0"/>
+        <v>8.6999999999999994E-3</v>
+      </c>
+      <c r="W7" s="1">
+        <f t="shared" si="1"/>
+        <v>7.466863875283068E-3</v>
+      </c>
     </row>
-    <row r="8" spans="1:23">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1200</v>
       </c>
       <c r="B8" s="1">
@@ -15903,10 +17243,18 @@
       <c r="U8" s="1">
         <v>4.7549999999999997E-3</v>
       </c>
+      <c r="V8" s="1">
+        <f t="shared" si="0"/>
+        <v>1.2528000000000001E-2</v>
+      </c>
+      <c r="W8" s="1">
+        <f t="shared" si="1"/>
+        <v>1.3245501898696924E-2</v>
+      </c>
     </row>
-    <row r="9" spans="1:23">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1400</v>
       </c>
       <c r="B9" s="1">
@@ -15969,10 +17317,18 @@
       <c r="U9" s="1">
         <v>6.8669999999999998E-3</v>
       </c>
+      <c r="V9" s="1">
+        <f t="shared" si="0"/>
+        <v>1.7052000000000001E-2</v>
+      </c>
+      <c r="W9" s="1">
+        <f t="shared" si="1"/>
+        <v>2.1493229187816539E-2</v>
+      </c>
     </row>
-    <row r="10" spans="1:23">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1600</v>
       </c>
       <c r="B10" s="1">
@@ -16035,10 +17391,18 @@
       <c r="U10" s="1">
         <v>9.4839999999999994E-3</v>
       </c>
+      <c r="V10" s="1">
+        <f t="shared" si="0"/>
+        <v>2.2272E-2</v>
+      </c>
+      <c r="W10" s="1">
+        <f t="shared" si="1"/>
+        <v>3.2677490011103587E-2</v>
+      </c>
     </row>
-    <row r="11" spans="1:23">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1800</v>
       </c>
       <c r="B11" s="1">
@@ -16101,10 +17465,18 @@
       <c r="U11" s="1">
         <v>1.2292000000000001E-2</v>
       </c>
+      <c r="V11" s="1">
+        <f t="shared" si="0"/>
+        <v>2.8188000000000001E-2</v>
+      </c>
+      <c r="W11" s="1">
+        <f t="shared" si="1"/>
+        <v>4.7273201442088658E-2</v>
+      </c>
     </row>
-    <row r="12" spans="1:23">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2000</v>
       </c>
       <c r="B12" s="1">
@@ -16167,10 +17539,18 @@
       <c r="U12" s="1">
         <v>1.5559999999999999E-2</v>
       </c>
+      <c r="V12" s="1">
+        <f t="shared" si="0"/>
+        <v>3.4799999999999998E-2</v>
+      </c>
+      <c r="W12" s="1">
+        <f t="shared" si="1"/>
+        <v>6.5761808355118523E-2</v>
+      </c>
     </row>
-    <row r="13" spans="1:23">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2200</v>
       </c>
       <c r="B13" s="1">
@@ -16233,10 +17613,18 @@
       <c r="U13" s="1">
         <v>1.9904999999999999E-2</v>
       </c>
+      <c r="V13" s="1">
+        <f t="shared" si="0"/>
+        <v>4.2108E-2</v>
+      </c>
+      <c r="W13" s="1">
+        <f t="shared" si="1"/>
+        <v>8.8630551503233859E-2</v>
+      </c>
     </row>
-    <row r="14" spans="1:23">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2400</v>
       </c>
       <c r="B14" s="1">
@@ -16299,10 +17687,18 @@
       <c r="U14" s="1">
         <v>2.4892000000000001E-2</v>
       </c>
+      <c r="V14" s="1">
+        <f t="shared" si="0"/>
+        <v>5.0112000000000004E-2</v>
+      </c>
+      <c r="W14" s="1">
+        <f t="shared" si="1"/>
+        <v>0.11637188368631836</v>
+      </c>
     </row>
-    <row r="15" spans="1:23">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2600</v>
       </c>
       <c r="B15" s="1">
@@ -16365,10 +17761,18 @@
       <c r="U15" s="1">
         <v>3.1033999999999999E-2</v>
       </c>
+      <c r="V15" s="1">
+        <f t="shared" si="0"/>
+        <v>5.8812000000000003E-2</v>
+      </c>
+      <c r="W15" s="1">
+        <f t="shared" si="1"/>
+        <v>0.14948299307789317</v>
+      </c>
     </row>
-    <row r="16" spans="1:23">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2800</v>
       </c>
       <c r="B16" s="1">
@@ -16431,10 +17835,18 @@
       <c r="U16" s="1">
         <v>3.6332999999999997E-2</v>
       </c>
+      <c r="V16" s="1">
+        <f t="shared" si="0"/>
+        <v>6.8208000000000005E-2</v>
+      </c>
+      <c r="W16" s="1">
+        <f t="shared" si="1"/>
+        <v>0.18846540662386987</v>
+      </c>
     </row>
-    <row r="17" spans="1:21">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3000</v>
       </c>
       <c r="B17" s="1">
@@ -16497,10 +17909,18 @@
       <c r="U17" s="1">
         <v>4.2215000000000003E-2</v>
       </c>
+      <c r="V17" s="1">
+        <f t="shared" si="0"/>
+        <v>7.8299999999999995E-2</v>
+      </c>
+      <c r="W17" s="1">
+        <f t="shared" si="1"/>
+        <v>0.23382465486320933</v>
+      </c>
     </row>
-    <row r="18" spans="1:21">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3200</v>
       </c>
       <c r="B18" s="1">
@@ -16563,10 +17983,18 @@
       <c r="U18" s="1">
         <v>4.8552999999999999E-2</v>
       </c>
+      <c r="V18" s="1">
+        <f t="shared" si="0"/>
+        <v>8.9088000000000001E-2</v>
+      </c>
+      <c r="W18" s="1">
+        <f t="shared" si="1"/>
+        <v>0.28606998490436619</v>
+      </c>
     </row>
-    <row r="19" spans="1:21">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3400</v>
       </c>
       <c r="B19" s="1">
@@ -16629,10 +18057,18 @@
       <c r="U19" s="1">
         <v>5.6797E-2</v>
       </c>
+      <c r="V19" s="1">
+        <f t="shared" si="0"/>
+        <v>0.10057200000000001</v>
+      </c>
+      <c r="W19" s="1">
+        <f t="shared" si="1"/>
+        <v>0.34571411186055784</v>
+      </c>
     </row>
-    <row r="20" spans="1:21">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3600</v>
       </c>
       <c r="B20" s="1">
@@ -16695,10 +18131,18 @@
       <c r="U20" s="1">
         <v>6.3672999999999993E-2</v>
       </c>
+      <c r="V20" s="1">
+        <f t="shared" si="0"/>
+        <v>0.112752</v>
+      </c>
+      <c r="W20" s="1">
+        <f t="shared" si="1"/>
+        <v>0.41327300148988788</v>
+      </c>
     </row>
-    <row r="21" spans="1:21">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3800</v>
       </c>
       <c r="B21" s="1">
@@ -16761,10 +18205,18 @@
       <c r="U21" s="1">
         <v>7.1920999999999999E-2</v>
       </c>
+      <c r="V21" s="1">
+        <f t="shared" si="0"/>
+        <v>0.12562799999999999</v>
+      </c>
+      <c r="W21" s="1">
+        <f t="shared" si="1"/>
+        <v>0.48926567850474051</v>
+      </c>
     </row>
-    <row r="22" spans="1:21">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>4000</v>
       </c>
       <c r="B22" s="1">
@@ -16827,904 +18279,912 @@
       <c r="U22" s="1">
         <v>8.1115000000000007E-2</v>
       </c>
+      <c r="V22" s="1">
+        <f t="shared" si="0"/>
+        <v>0.13919999999999999</v>
+      </c>
+      <c r="W22" s="1">
+        <f t="shared" si="1"/>
+        <v>0.57421405625236421</v>
+      </c>
     </row>
-    <row r="25" spans="1:21">
-      <c r="I25" s="3" t="s">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="I25" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="J25" s="3"/>
-      <c r="K25" s="3"/>
+      <c r="J25" s="6"/>
+      <c r="K25" s="6"/>
     </row>
-    <row r="26" spans="1:21">
-      <c r="I26" s="3"/>
-      <c r="J26" s="3"/>
-      <c r="K26" s="3"/>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="I26" s="6"/>
+      <c r="J26" s="6"/>
+      <c r="K26" s="6"/>
     </row>
-    <row r="27" spans="1:21">
-      <c r="I27" s="3"/>
-      <c r="J27" s="3"/>
-      <c r="K27" s="3"/>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="I27" s="6"/>
+      <c r="J27" s="6"/>
+      <c r="K27" s="6"/>
     </row>
-    <row r="28" spans="1:21">
-      <c r="I28" s="3"/>
-      <c r="J28" s="3"/>
-      <c r="K28" s="3"/>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="I28" s="6"/>
+      <c r="J28" s="6"/>
+      <c r="K28" s="6"/>
     </row>
-    <row r="54" spans="3:8">
-      <c r="C54" s="7"/>
-      <c r="D54" s="7" t="s">
+    <row r="54" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C54" s="3"/>
+      <c r="D54" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E54" s="7"/>
-      <c r="F54" s="7"/>
-      <c r="G54" s="7" t="s">
+      <c r="E54" s="3"/>
+      <c r="F54" s="3"/>
+      <c r="G54" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H54" s="7"/>
+      <c r="H54" s="3"/>
     </row>
-    <row r="55" spans="3:8">
-      <c r="C55" s="7"/>
-      <c r="D55" s="7"/>
-      <c r="E55" s="7"/>
-      <c r="F55" s="7"/>
-      <c r="G55" s="7"/>
-      <c r="H55" s="7"/>
+    <row r="55" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C55" s="3"/>
+      <c r="D55" s="3"/>
+      <c r="E55" s="3"/>
+      <c r="F55" s="3"/>
+      <c r="G55" s="3"/>
+      <c r="H55" s="3"/>
     </row>
-    <row r="56" spans="3:8">
-      <c r="C56" s="7"/>
-      <c r="D56" s="7" t="s">
+    <row r="56" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C56" s="3"/>
+      <c r="D56" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E56" s="7"/>
-      <c r="F56" s="7"/>
-      <c r="G56" s="7" t="s">
+      <c r="E56" s="3"/>
+      <c r="F56" s="3"/>
+      <c r="G56" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="H56" s="7"/>
+      <c r="H56" s="3"/>
     </row>
-    <row r="57" spans="3:8">
-      <c r="C57" s="7"/>
-      <c r="D57" s="7">
+    <row r="57" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C57" s="3"/>
+      <c r="D57" s="3">
         <v>0.14348</v>
       </c>
-      <c r="E57" s="7">
+      <c r="E57" s="3">
         <v>0.36096299999999998</v>
       </c>
-      <c r="F57" s="7"/>
-      <c r="G57" s="7">
+      <c r="F57" s="3"/>
+      <c r="G57" s="3">
         <v>0.35458400000000001</v>
       </c>
-      <c r="H57" s="7">
+      <c r="H57" s="3">
         <v>0.90989399999999998</v>
       </c>
     </row>
-    <row r="58" spans="3:8">
-      <c r="C58" s="7"/>
-      <c r="D58" s="7">
+    <row r="58" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C58" s="3"/>
+      <c r="D58" s="3">
         <v>0.15925</v>
       </c>
-      <c r="E58" s="7">
+      <c r="E58" s="3">
         <v>0.41607</v>
       </c>
-      <c r="F58" s="7"/>
-      <c r="G58" s="7">
+      <c r="F58" s="3"/>
+      <c r="G58" s="3">
         <v>0.392876</v>
       </c>
-      <c r="H58" s="7">
+      <c r="H58" s="3">
         <v>0.98537200000000003</v>
       </c>
     </row>
-    <row r="59" spans="3:8">
-      <c r="C59" s="7"/>
-      <c r="D59" s="7">
+    <row r="59" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C59" s="3"/>
+      <c r="D59" s="3">
         <v>0.17818999999999999</v>
       </c>
-      <c r="E59" s="7">
+      <c r="E59" s="3">
         <v>0.45431300000000002</v>
       </c>
-      <c r="F59" s="7"/>
-      <c r="G59" s="7">
+      <c r="F59" s="3"/>
+      <c r="G59" s="3">
         <v>0.42042600000000002</v>
       </c>
-      <c r="H59" s="7">
+      <c r="H59" s="3">
         <v>1.06596</v>
       </c>
     </row>
-    <row r="60" spans="3:8">
-      <c r="C60" s="7"/>
-      <c r="D60" s="7">
+    <row r="60" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C60" s="3"/>
+      <c r="D60" s="3">
         <v>0.19994500000000001</v>
       </c>
-      <c r="E60" s="7">
+      <c r="E60" s="3">
         <v>0.50465700000000002</v>
       </c>
-      <c r="F60" s="7"/>
-      <c r="G60" s="7">
+      <c r="F60" s="3"/>
+      <c r="G60" s="3">
         <v>0.45450299999999999</v>
       </c>
-      <c r="H60" s="7">
+      <c r="H60" s="3">
         <v>1.139864</v>
       </c>
     </row>
-    <row r="61" spans="3:8">
-      <c r="C61" s="7"/>
-      <c r="D61" s="7">
+    <row r="61" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C61" s="3"/>
+      <c r="D61" s="3">
         <v>0.220527</v>
       </c>
-      <c r="E61" s="7">
+      <c r="E61" s="3">
         <v>0.55822300000000002</v>
       </c>
-      <c r="F61" s="7"/>
-      <c r="G61" s="7">
+      <c r="F61" s="3"/>
+      <c r="G61" s="3">
         <v>0.48921999999999999</v>
       </c>
-      <c r="H61" s="7">
+      <c r="H61" s="3">
         <v>1.2165900000000001</v>
       </c>
     </row>
-    <row r="62" spans="3:8">
-      <c r="C62" s="7"/>
-      <c r="D62" s="7">
+    <row r="62" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C62" s="3"/>
+      <c r="D62" s="3">
         <v>0.244924</v>
       </c>
-      <c r="E62" s="7">
+      <c r="E62" s="3">
         <v>0.61022299999999996</v>
       </c>
-      <c r="F62" s="7"/>
-      <c r="G62" s="7">
+      <c r="F62" s="3"/>
+      <c r="G62" s="3">
         <v>0.51994700000000005</v>
       </c>
-      <c r="H62" s="7">
+      <c r="H62" s="3">
         <v>1.310902</v>
       </c>
     </row>
-    <row r="63" spans="3:8">
-      <c r="C63" s="7"/>
-      <c r="D63" s="7">
+    <row r="63" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C63" s="3"/>
+      <c r="D63" s="3">
         <v>0.26701000000000003</v>
       </c>
-      <c r="E63" s="7">
+      <c r="E63" s="3">
         <v>0.66588499999999995</v>
       </c>
-      <c r="F63" s="7"/>
-      <c r="G63" s="7" t="s">
+      <c r="F63" s="3"/>
+      <c r="G63" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H63" s="7"/>
+      <c r="H63" s="3"/>
     </row>
-    <row r="64" spans="3:8">
-      <c r="C64" s="7"/>
-      <c r="D64" s="7">
+    <row r="64" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C64" s="3"/>
+      <c r="D64" s="3">
         <v>0.29008499999999998</v>
       </c>
-      <c r="E64" s="7">
+      <c r="E64" s="3">
         <v>0.72476200000000002</v>
       </c>
-      <c r="F64" s="7"/>
-      <c r="G64" s="7">
+      <c r="F64" s="3"/>
+      <c r="G64" s="3">
         <v>0.36982100000000001</v>
       </c>
-      <c r="H64" s="7">
+      <c r="H64" s="3">
         <v>0.95696499999999995</v>
       </c>
     </row>
-    <row r="65" spans="3:8">
-      <c r="C65" s="7"/>
-      <c r="D65" s="7">
+    <row r="65" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C65" s="3"/>
+      <c r="D65" s="3">
         <v>0.317388</v>
       </c>
-      <c r="E65" s="7">
+      <c r="E65" s="3">
         <v>0.788995</v>
       </c>
-      <c r="F65" s="7"/>
-      <c r="G65" s="7">
+      <c r="F65" s="3"/>
+      <c r="G65" s="3">
         <v>0.397484</v>
       </c>
-      <c r="H65" s="7">
+      <c r="H65" s="3">
         <v>1.000964</v>
       </c>
     </row>
-    <row r="66" spans="3:8">
-      <c r="C66" s="7"/>
-      <c r="D66" s="7">
+    <row r="66" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C66" s="3"/>
+      <c r="D66" s="3">
         <v>0.344225</v>
       </c>
-      <c r="E66" s="7">
+      <c r="E66" s="3">
         <v>0.85274300000000003</v>
       </c>
-      <c r="F66" s="7"/>
-      <c r="G66" s="7">
+      <c r="F66" s="3"/>
+      <c r="G66" s="3">
         <v>0.42614800000000003</v>
       </c>
-      <c r="H66" s="7">
+      <c r="H66" s="3">
         <v>1.0664960000000001</v>
       </c>
     </row>
-    <row r="67" spans="3:8">
-      <c r="C67" s="7"/>
-      <c r="D67" s="7">
+    <row r="67" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C67" s="3"/>
+      <c r="D67" s="3">
         <v>0.37059300000000001</v>
       </c>
-      <c r="E67" s="7">
+      <c r="E67" s="3">
         <v>0.91947299999999998</v>
       </c>
-      <c r="F67" s="7"/>
-      <c r="G67" s="7">
+      <c r="F67" s="3"/>
+      <c r="G67" s="3">
         <v>0.46109600000000001</v>
       </c>
-      <c r="H67" s="7">
+      <c r="H67" s="3">
         <v>1.1387640000000001</v>
       </c>
     </row>
-    <row r="68" spans="3:8">
-      <c r="C68" s="7"/>
-      <c r="D68" s="7" t="s">
+    <row r="68" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C68" s="3"/>
+      <c r="D68" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E68" s="7"/>
-      <c r="F68" s="7"/>
-      <c r="G68" s="7">
+      <c r="E68" s="3"/>
+      <c r="F68" s="3"/>
+      <c r="G68" s="3">
         <v>0.49199799999999999</v>
       </c>
-      <c r="H68" s="7">
+      <c r="H68" s="3">
         <v>1.214129</v>
       </c>
     </row>
-    <row r="69" spans="3:8">
-      <c r="C69" s="7"/>
-      <c r="D69" s="7">
+    <row r="69" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C69" s="3"/>
+      <c r="D69" s="3">
         <v>0.14651500000000001</v>
       </c>
-      <c r="E69" s="7">
+      <c r="E69" s="3">
         <v>0.38476199999999999</v>
       </c>
-      <c r="F69" s="7"/>
-      <c r="G69" s="7">
+      <c r="F69" s="3"/>
+      <c r="G69" s="3">
         <v>0.52045300000000005</v>
       </c>
-      <c r="H69" s="7">
+      <c r="H69" s="3">
         <v>1.3863760000000001</v>
       </c>
     </row>
-    <row r="70" spans="3:8">
-      <c r="C70" s="7"/>
-      <c r="D70" s="7">
+    <row r="70" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C70" s="3"/>
+      <c r="D70" s="3">
         <v>0.16389699999999999</v>
       </c>
-      <c r="E70" s="7">
+      <c r="E70" s="3">
         <v>0.423433</v>
       </c>
-      <c r="F70" s="7"/>
-      <c r="G70" s="7" t="s">
+      <c r="F70" s="3"/>
+      <c r="G70" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H70" s="7"/>
+      <c r="H70" s="3"/>
     </row>
-    <row r="71" spans="3:8">
-      <c r="C71" s="7"/>
-      <c r="D71" s="7">
+    <row r="71" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C71" s="3"/>
+      <c r="D71" s="3">
         <v>0.17909</v>
       </c>
-      <c r="E71" s="7">
+      <c r="E71" s="3">
         <v>0.47237000000000001</v>
       </c>
-      <c r="F71" s="7"/>
-      <c r="G71" s="7">
+      <c r="F71" s="3"/>
+      <c r="G71" s="3">
         <v>0.36776300000000001</v>
       </c>
-      <c r="H71" s="7">
+      <c r="H71" s="3">
         <v>0.912547</v>
       </c>
     </row>
-    <row r="72" spans="3:8">
-      <c r="C72" s="7"/>
-      <c r="D72" s="7">
+    <row r="72" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C72" s="3"/>
+      <c r="D72" s="3">
         <v>0.19886499999999999</v>
       </c>
-      <c r="E72" s="7">
+      <c r="E72" s="3">
         <v>0.52192799999999995</v>
       </c>
-      <c r="F72" s="7"/>
-      <c r="G72" s="7">
+      <c r="F72" s="3"/>
+      <c r="G72" s="3">
         <v>0.40051900000000001</v>
       </c>
-      <c r="H72" s="7">
+      <c r="H72" s="3">
         <v>0.99871100000000002</v>
       </c>
     </row>
-    <row r="73" spans="3:8">
-      <c r="C73" s="7"/>
-      <c r="D73" s="7">
+    <row r="73" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C73" s="3"/>
+      <c r="D73" s="3">
         <v>0.21914900000000001</v>
       </c>
-      <c r="E73" s="7">
+      <c r="E73" s="3">
         <v>0.57533800000000002</v>
       </c>
-      <c r="F73" s="7"/>
-      <c r="G73" s="7">
+      <c r="F73" s="3"/>
+      <c r="G73" s="3">
         <v>0.43451899999999999</v>
       </c>
-      <c r="H73" s="7">
+      <c r="H73" s="3">
         <v>1.0066250000000001</v>
       </c>
     </row>
-    <row r="74" spans="3:8">
-      <c r="C74" s="7"/>
-      <c r="D74" s="7">
+    <row r="74" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C74" s="3"/>
+      <c r="D74" s="3">
         <v>0.242121</v>
       </c>
-      <c r="E74" s="7">
+      <c r="E74" s="3">
         <v>0.63816899999999999</v>
       </c>
-      <c r="F74" s="7"/>
-      <c r="G74" s="7">
+      <c r="F74" s="3"/>
+      <c r="G74" s="3">
         <v>0.46414</v>
       </c>
-      <c r="H74" s="7">
+      <c r="H74" s="3">
         <v>1.0740670000000001</v>
       </c>
     </row>
-    <row r="75" spans="3:8">
-      <c r="C75" s="7"/>
-      <c r="D75" s="7">
+    <row r="75" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C75" s="3"/>
+      <c r="D75" s="3">
         <v>0.326405</v>
       </c>
-      <c r="E75" s="7">
+      <c r="E75" s="3">
         <v>0.68771700000000002</v>
       </c>
-      <c r="F75" s="7"/>
-      <c r="G75" s="7">
+      <c r="F75" s="3"/>
+      <c r="G75" s="3">
         <v>0.497643</v>
       </c>
-      <c r="H75" s="7">
+      <c r="H75" s="3">
         <v>1.2994939999999999</v>
       </c>
     </row>
-    <row r="76" spans="3:8">
-      <c r="C76" s="7"/>
-      <c r="D76" s="7">
+    <row r="76" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C76" s="3"/>
+      <c r="D76" s="3">
         <v>0.293018</v>
       </c>
-      <c r="E76" s="7">
+      <c r="E76" s="3">
         <v>0.73973699999999998</v>
       </c>
-      <c r="F76" s="7"/>
-      <c r="G76" s="7">
+      <c r="F76" s="3"/>
+      <c r="G76" s="3">
         <v>0.54237000000000002</v>
       </c>
-      <c r="H76" s="7">
+      <c r="H76" s="3">
         <v>1.224828</v>
       </c>
     </row>
-    <row r="77" spans="3:8">
-      <c r="C77" s="7"/>
-      <c r="D77" s="7">
+    <row r="77" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C77" s="3"/>
+      <c r="D77" s="3">
         <v>0.320052</v>
       </c>
-      <c r="E77" s="7">
+      <c r="E77" s="3">
         <v>0.80922400000000005</v>
       </c>
-      <c r="F77" s="7"/>
-      <c r="G77" s="7" t="s">
+      <c r="F77" s="3"/>
+      <c r="G77" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H77" s="7"/>
+      <c r="H77" s="3"/>
     </row>
-    <row r="78" spans="3:8">
-      <c r="C78" s="7"/>
-      <c r="D78" s="7">
+    <row r="78" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C78" s="3"/>
+      <c r="D78" s="3">
         <v>0.34369499999999997</v>
       </c>
-      <c r="E78" s="7">
+      <c r="E78" s="3">
         <v>0.86548499999999995</v>
       </c>
-      <c r="F78" s="7"/>
-      <c r="G78" s="7">
+      <c r="F78" s="3"/>
+      <c r="G78" s="3">
         <v>0.38773400000000002</v>
       </c>
-      <c r="H78" s="7">
+      <c r="H78" s="3">
         <v>0.81385399999999997</v>
       </c>
     </row>
-    <row r="79" spans="3:8">
-      <c r="C79" s="7"/>
-      <c r="D79" s="7">
+    <row r="79" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C79" s="3"/>
+      <c r="D79" s="3">
         <v>0.37206800000000001</v>
       </c>
-      <c r="E79" s="7">
+      <c r="E79" s="3">
         <v>0.93661099999999997</v>
       </c>
-      <c r="F79" s="7"/>
-      <c r="G79" s="7">
+      <c r="F79" s="3"/>
+      <c r="G79" s="3">
         <v>0.40659299999999998</v>
       </c>
-      <c r="H79" s="7">
+      <c r="H79" s="3">
         <v>0.86788799999999999</v>
       </c>
     </row>
-    <row r="80" spans="3:8">
-      <c r="C80" s="7"/>
-      <c r="D80" s="7" t="s">
+    <row r="80" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C80" s="3"/>
+      <c r="D80" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E80" s="7"/>
-      <c r="F80" s="7"/>
-      <c r="G80" s="7">
+      <c r="E80" s="3"/>
+      <c r="F80" s="3"/>
+      <c r="G80" s="3">
         <v>0.44289299999999998</v>
       </c>
-      <c r="H80" s="7">
+      <c r="H80" s="3">
         <v>0.92518500000000004</v>
       </c>
     </row>
-    <row r="81" spans="3:8">
-      <c r="C81" s="7"/>
-      <c r="D81" s="7">
+    <row r="81" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C81" s="3"/>
+      <c r="D81" s="3">
         <v>0.14693600000000001</v>
       </c>
-      <c r="E81" s="7">
+      <c r="E81" s="3">
         <v>0.364479</v>
       </c>
-      <c r="F81" s="7"/>
-      <c r="G81" s="7">
+      <c r="F81" s="3"/>
+      <c r="G81" s="3">
         <v>0.47003499999999998</v>
       </c>
-      <c r="H81" s="7">
+      <c r="H81" s="3">
         <v>0.99759900000000001</v>
       </c>
     </row>
-    <row r="82" spans="3:8">
-      <c r="C82" s="7"/>
-      <c r="D82" s="7">
+    <row r="82" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C82" s="3"/>
+      <c r="D82" s="3">
         <v>0.16577800000000001</v>
       </c>
-      <c r="E82" s="7">
+      <c r="E82" s="3">
         <v>0.39681</v>
       </c>
-      <c r="F82" s="7"/>
-      <c r="G82" s="7">
+      <c r="F82" s="3"/>
+      <c r="G82" s="3">
         <v>0.50515900000000002</v>
       </c>
-      <c r="H82" s="7">
+      <c r="H82" s="3">
         <v>1.0538989999999999</v>
       </c>
     </row>
-    <row r="83" spans="3:8">
-      <c r="C83" s="7"/>
-      <c r="D83" s="7">
+    <row r="83" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C83" s="3"/>
+      <c r="D83" s="3">
         <v>0.18443100000000001</v>
       </c>
-      <c r="E83" s="7">
+      <c r="E83" s="3">
         <v>0.44147799999999998</v>
       </c>
-      <c r="F83" s="7"/>
-      <c r="G83" s="7">
+      <c r="F83" s="3"/>
+      <c r="G83" s="3">
         <v>0.53899799999999998</v>
       </c>
-      <c r="H83" s="7">
+      <c r="H83" s="3">
         <v>1.1230150000000001</v>
       </c>
     </row>
-    <row r="84" spans="3:8">
-      <c r="C84" s="7"/>
-      <c r="D84" s="7">
+    <row r="84" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C84" s="3"/>
+      <c r="D84" s="3">
         <v>0.20438799999999999</v>
       </c>
-      <c r="E84" s="7">
+      <c r="E84" s="3">
         <v>0.48889700000000003</v>
       </c>
-      <c r="F84" s="7"/>
-      <c r="G84" s="7" t="s">
+      <c r="F84" s="3"/>
+      <c r="G84" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H84" s="7"/>
+      <c r="H84" s="3"/>
     </row>
-    <row r="85" spans="3:8">
-      <c r="C85" s="7"/>
-      <c r="D85" s="7">
+    <row r="85" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C85" s="3"/>
+      <c r="D85" s="3">
         <v>0.22651399999999999</v>
       </c>
-      <c r="E85" s="7">
+      <c r="E85" s="3">
         <v>0.53690000000000004</v>
       </c>
-      <c r="F85" s="7"/>
-      <c r="G85" s="7">
+      <c r="F85" s="3"/>
+      <c r="G85" s="3">
         <v>0.38480999999999999</v>
       </c>
-      <c r="H85" s="7">
+      <c r="H85" s="3">
         <v>0.70749700000000004</v>
       </c>
     </row>
-    <row r="86" spans="3:8">
-      <c r="C86" s="7"/>
-      <c r="D86" s="7">
+    <row r="86" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C86" s="3"/>
+      <c r="D86" s="3">
         <v>0.24813399999999999</v>
       </c>
-      <c r="E86" s="7">
+      <c r="E86" s="3">
         <v>0.586426</v>
       </c>
-      <c r="F86" s="7"/>
-      <c r="G86" s="7">
+      <c r="F86" s="3"/>
+      <c r="G86" s="3">
         <v>0.41434399999999999</v>
       </c>
-      <c r="H86" s="7">
+      <c r="H86" s="3">
         <v>0.755463</v>
       </c>
     </row>
-    <row r="87" spans="3:8">
-      <c r="C87" s="7"/>
-      <c r="D87" s="7">
+    <row r="87" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C87" s="3"/>
+      <c r="D87" s="3">
         <v>0.27271800000000002</v>
       </c>
-      <c r="E87" s="7">
+      <c r="E87" s="3">
         <v>0.64016200000000001</v>
       </c>
-      <c r="F87" s="7"/>
-      <c r="G87" s="7">
+      <c r="F87" s="3"/>
+      <c r="G87" s="3">
         <v>0.445884</v>
       </c>
-      <c r="H87" s="7">
+      <c r="H87" s="3">
         <v>0.80748500000000001</v>
       </c>
     </row>
-    <row r="88" spans="3:8">
-      <c r="C88" s="7"/>
-      <c r="D88" s="7">
+    <row r="88" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C88" s="3"/>
+      <c r="D88" s="3">
         <v>0.296153</v>
       </c>
-      <c r="E88" s="7">
+      <c r="E88" s="3">
         <v>0.69698700000000002</v>
       </c>
-      <c r="F88" s="7"/>
-      <c r="G88" s="7">
+      <c r="F88" s="3"/>
+      <c r="G88" s="3">
         <v>0.47498099999999999</v>
       </c>
-      <c r="H88" s="7">
+      <c r="H88" s="3">
         <v>0.86903799999999998</v>
       </c>
     </row>
-    <row r="89" spans="3:8">
-      <c r="C89" s="7"/>
-      <c r="D89" s="7">
+    <row r="89" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C89" s="3"/>
+      <c r="D89" s="3">
         <v>0.32544899999999999</v>
       </c>
-      <c r="E89" s="7">
+      <c r="E89" s="3">
         <v>0.75214999999999999</v>
       </c>
-      <c r="F89" s="7"/>
-      <c r="G89" s="7">
+      <c r="F89" s="3"/>
+      <c r="G89" s="3">
         <v>0.48132200000000003</v>
       </c>
-      <c r="H89" s="7">
+      <c r="H89" s="3">
         <v>0.92292600000000002</v>
       </c>
     </row>
-    <row r="90" spans="3:8">
-      <c r="C90" s="7"/>
-      <c r="D90" s="7">
+    <row r="90" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C90" s="3"/>
+      <c r="D90" s="3">
         <v>0.34912900000000002</v>
       </c>
-      <c r="E90" s="7">
+      <c r="E90" s="3">
         <v>0.81225400000000003</v>
       </c>
-      <c r="F90" s="7"/>
-      <c r="G90" s="7">
+      <c r="F90" s="3"/>
+      <c r="G90" s="3">
         <v>0.54292600000000002</v>
       </c>
-      <c r="H90" s="7">
+      <c r="H90" s="3">
         <v>0.98124999999999996</v>
       </c>
     </row>
-    <row r="91" spans="3:8">
-      <c r="C91" s="7"/>
-      <c r="D91" s="7">
+    <row r="91" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C91" s="3"/>
+      <c r="D91" s="3">
         <v>0.37545499999999998</v>
       </c>
-      <c r="E91" s="7">
+      <c r="E91" s="3">
         <v>0.87400999999999995</v>
       </c>
-      <c r="F91" s="7"/>
-      <c r="G91" s="7"/>
-      <c r="H91" s="7"/>
+      <c r="F91" s="3"/>
+      <c r="G91" s="3"/>
+      <c r="H91" s="3"/>
     </row>
-    <row r="92" spans="3:8">
-      <c r="C92" s="7"/>
-      <c r="D92" s="7" t="s">
+    <row r="92" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C92" s="3"/>
+      <c r="D92" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E92" s="7"/>
-      <c r="F92" s="7"/>
-      <c r="G92" s="7"/>
-      <c r="H92" s="7"/>
+      <c r="E92" s="3"/>
+      <c r="F92" s="3"/>
+      <c r="G92" s="3"/>
+      <c r="H92" s="3"/>
     </row>
-    <row r="93" spans="3:8">
-      <c r="C93" s="7"/>
-      <c r="D93" s="7">
+    <row r="93" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C93" s="3"/>
+      <c r="D93" s="3">
         <v>0.148142</v>
       </c>
-      <c r="E93" s="7">
+      <c r="E93" s="3">
         <v>0.33201000000000003</v>
       </c>
-      <c r="F93" s="7"/>
-      <c r="G93" s="7"/>
-      <c r="H93" s="7"/>
+      <c r="F93" s="3"/>
+      <c r="G93" s="3"/>
+      <c r="H93" s="3"/>
     </row>
-    <row r="94" spans="3:8">
-      <c r="C94" s="7"/>
-      <c r="D94" s="7">
+    <row r="94" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C94" s="3"/>
+      <c r="D94" s="3">
         <v>0.165737</v>
       </c>
-      <c r="E94" s="7">
+      <c r="E94" s="3">
         <v>0.36475400000000002</v>
       </c>
-      <c r="F94" s="7"/>
-      <c r="G94" s="7"/>
-      <c r="H94" s="7"/>
+      <c r="F94" s="3"/>
+      <c r="G94" s="3"/>
+      <c r="H94" s="3"/>
     </row>
-    <row r="95" spans="3:8">
-      <c r="C95" s="7"/>
-      <c r="D95" s="7">
+    <row r="95" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C95" s="3"/>
+      <c r="D95" s="3">
         <v>0.19029699999999999</v>
       </c>
-      <c r="E95" s="7">
+      <c r="E95" s="3">
         <v>0.40659200000000001</v>
       </c>
-      <c r="F95" s="7"/>
-      <c r="G95" s="7"/>
-      <c r="H95" s="7"/>
+      <c r="F95" s="3"/>
+      <c r="G95" s="3"/>
+      <c r="H95" s="3"/>
     </row>
-    <row r="96" spans="3:8">
-      <c r="C96" s="7"/>
-      <c r="D96" s="7">
+    <row r="96" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C96" s="3"/>
+      <c r="D96" s="3">
         <v>0.206178</v>
       </c>
-      <c r="E96" s="7">
+      <c r="E96" s="3">
         <v>0.45174300000000001</v>
       </c>
-      <c r="F96" s="7"/>
-      <c r="G96" s="7"/>
-      <c r="H96" s="7"/>
+      <c r="F96" s="3"/>
+      <c r="G96" s="3"/>
+      <c r="H96" s="3"/>
     </row>
-    <row r="97" spans="3:8">
-      <c r="C97" s="7"/>
-      <c r="D97" s="7">
+    <row r="97" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C97" s="3"/>
+      <c r="D97" s="3">
         <v>0.22791700000000001</v>
       </c>
-      <c r="E97" s="7">
+      <c r="E97" s="3">
         <v>0.496894</v>
       </c>
-      <c r="F97" s="7"/>
-      <c r="G97" s="7"/>
-      <c r="H97" s="7"/>
+      <c r="F97" s="3"/>
+      <c r="G97" s="3"/>
+      <c r="H97" s="3"/>
     </row>
-    <row r="98" spans="3:8">
-      <c r="C98" s="7"/>
-      <c r="D98" s="7">
+    <row r="98" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C98" s="3"/>
+      <c r="D98" s="3">
         <v>0.25129099999999999</v>
       </c>
-      <c r="E98" s="7">
+      <c r="E98" s="3">
         <v>0.54199399999999998</v>
       </c>
-      <c r="F98" s="7"/>
-      <c r="G98" s="7"/>
-      <c r="H98" s="7"/>
+      <c r="F98" s="3"/>
+      <c r="G98" s="3"/>
+      <c r="H98" s="3"/>
     </row>
-    <row r="99" spans="3:8">
-      <c r="C99" s="7"/>
-      <c r="D99" s="7">
+    <row r="99" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C99" s="3"/>
+      <c r="D99" s="3">
         <v>0.273343</v>
       </c>
-      <c r="E99" s="7">
+      <c r="E99" s="3">
         <v>0.59726100000000004</v>
       </c>
-      <c r="F99" s="7"/>
-      <c r="G99" s="7"/>
-      <c r="H99" s="7"/>
+      <c r="F99" s="3"/>
+      <c r="G99" s="3"/>
+      <c r="H99" s="3"/>
     </row>
-    <row r="100" spans="3:8">
-      <c r="C100" s="7"/>
-      <c r="D100" s="7">
+    <row r="100" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C100" s="3"/>
+      <c r="D100" s="3">
         <v>0.29266300000000001</v>
       </c>
-      <c r="E100" s="7">
+      <c r="E100" s="3">
         <v>0.64127100000000004</v>
       </c>
-      <c r="F100" s="7"/>
-      <c r="G100" s="7"/>
-      <c r="H100" s="7"/>
+      <c r="F100" s="3"/>
+      <c r="G100" s="3"/>
+      <c r="H100" s="3"/>
     </row>
-    <row r="101" spans="3:8">
-      <c r="C101" s="7"/>
-      <c r="D101" s="7">
+    <row r="101" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C101" s="3"/>
+      <c r="D101" s="3">
         <v>0.31692900000000002</v>
       </c>
-      <c r="E101" s="7">
+      <c r="E101" s="3">
         <v>0.80818400000000001</v>
       </c>
-      <c r="F101" s="7"/>
-      <c r="G101" s="7"/>
-      <c r="H101" s="7"/>
+      <c r="F101" s="3"/>
+      <c r="G101" s="3"/>
+      <c r="H101" s="3"/>
     </row>
-    <row r="102" spans="3:8">
-      <c r="C102" s="7"/>
-      <c r="D102" s="7">
+    <row r="102" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C102" s="3"/>
+      <c r="D102" s="3">
         <v>0.37176500000000001</v>
       </c>
-      <c r="E102" s="7">
+      <c r="E102" s="3">
         <v>0.80840400000000001</v>
       </c>
-      <c r="F102" s="7"/>
-      <c r="G102" s="7"/>
-      <c r="H102" s="7"/>
+      <c r="F102" s="3"/>
+      <c r="G102" s="3"/>
+      <c r="H102" s="3"/>
     </row>
-    <row r="103" spans="3:8">
-      <c r="C103" s="7"/>
-      <c r="D103" s="7">
+    <row r="103" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C103" s="3"/>
+      <c r="D103" s="3">
         <v>0.36516700000000002</v>
       </c>
-      <c r="E103" s="7">
+      <c r="E103" s="3">
         <v>0.82933500000000004</v>
       </c>
-      <c r="F103" s="7"/>
-      <c r="G103" s="7"/>
-      <c r="H103" s="7"/>
+      <c r="F103" s="3"/>
+      <c r="G103" s="3"/>
+      <c r="H103" s="3"/>
     </row>
-    <row r="104" spans="3:8">
-      <c r="C104" s="7"/>
-      <c r="D104" s="7" t="s">
+    <row r="104" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C104" s="3"/>
+      <c r="D104" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E104" s="7"/>
-      <c r="F104" s="7"/>
-      <c r="G104" s="7"/>
-      <c r="H104" s="7"/>
+      <c r="E104" s="3"/>
+      <c r="F104" s="3"/>
+      <c r="G104" s="3"/>
+      <c r="H104" s="3"/>
     </row>
-    <row r="105" spans="3:8">
-      <c r="C105" s="7"/>
-      <c r="D105" s="7">
+    <row r="105" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C105" s="3"/>
+      <c r="D105" s="3">
         <v>0.14640300000000001</v>
       </c>
-      <c r="E105" s="7">
+      <c r="E105" s="3">
         <v>0.30193500000000001</v>
       </c>
-      <c r="F105" s="7"/>
-      <c r="G105" s="7"/>
-      <c r="H105" s="7"/>
+      <c r="F105" s="3"/>
+      <c r="G105" s="3"/>
+      <c r="H105" s="3"/>
     </row>
-    <row r="106" spans="3:8">
-      <c r="C106" s="7"/>
-      <c r="D106" s="7">
+    <row r="106" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C106" s="3"/>
+      <c r="D106" s="3">
         <v>0.16289799999999999</v>
       </c>
-      <c r="E106" s="7">
+      <c r="E106" s="3">
         <v>0.32373600000000002</v>
       </c>
-      <c r="F106" s="7"/>
-      <c r="G106" s="7"/>
-      <c r="H106" s="7"/>
+      <c r="F106" s="3"/>
+      <c r="G106" s="3"/>
+      <c r="H106" s="3"/>
     </row>
-    <row r="107" spans="3:8">
-      <c r="C107" s="7"/>
-      <c r="D107" s="7">
+    <row r="107" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C107" s="3"/>
+      <c r="D107" s="3">
         <v>0.18782199999999999</v>
       </c>
-      <c r="E107" s="7">
+      <c r="E107" s="3">
         <v>0.352354</v>
       </c>
-      <c r="F107" s="7"/>
-      <c r="G107" s="7"/>
-      <c r="H107" s="7"/>
+      <c r="F107" s="3"/>
+      <c r="G107" s="3"/>
+      <c r="H107" s="3"/>
     </row>
-    <row r="108" spans="3:8">
-      <c r="C108" s="7"/>
-      <c r="D108" s="7">
+    <row r="108" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C108" s="3"/>
+      <c r="D108" s="3">
         <v>0.20228499999999999</v>
       </c>
-      <c r="E108" s="7">
+      <c r="E108" s="3">
         <v>0.390102</v>
       </c>
-      <c r="F108" s="7"/>
-      <c r="G108" s="7"/>
-      <c r="H108" s="7"/>
+      <c r="F108" s="3"/>
+      <c r="G108" s="3"/>
+      <c r="H108" s="3"/>
     </row>
-    <row r="109" spans="3:8">
-      <c r="C109" s="7"/>
-      <c r="D109" s="7">
+    <row r="109" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C109" s="3"/>
+      <c r="D109" s="3">
         <v>0.22323000000000001</v>
       </c>
-      <c r="E109" s="7">
+      <c r="E109" s="3">
         <v>0.43582500000000002</v>
       </c>
-      <c r="F109" s="7"/>
-      <c r="G109" s="7"/>
-      <c r="H109" s="7"/>
+      <c r="F109" s="3"/>
+      <c r="G109" s="3"/>
+      <c r="H109" s="3"/>
     </row>
-    <row r="110" spans="3:8">
-      <c r="C110" s="7"/>
-      <c r="D110" s="7">
+    <row r="110" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C110" s="3"/>
+      <c r="D110" s="3">
         <v>0.24609200000000001</v>
       </c>
-      <c r="E110" s="7">
+      <c r="E110" s="3">
         <v>0.47254000000000002</v>
       </c>
-      <c r="F110" s="7"/>
-      <c r="G110" s="7"/>
-      <c r="H110" s="7"/>
+      <c r="F110" s="3"/>
+      <c r="G110" s="3"/>
+      <c r="H110" s="3"/>
     </row>
-    <row r="111" spans="3:8">
-      <c r="C111" s="7"/>
-      <c r="D111" s="7">
+    <row r="111" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C111" s="3"/>
+      <c r="D111" s="3">
         <v>0.26971800000000001</v>
       </c>
-      <c r="E111" s="7">
+      <c r="E111" s="3">
         <v>0.51329899999999995</v>
       </c>
-      <c r="F111" s="7"/>
-      <c r="G111" s="7"/>
-      <c r="H111" s="7"/>
+      <c r="F111" s="3"/>
+      <c r="G111" s="3"/>
+      <c r="H111" s="3"/>
     </row>
-    <row r="112" spans="3:8">
-      <c r="C112" s="7"/>
-      <c r="D112" s="7">
+    <row r="112" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C112" s="3"/>
+      <c r="D112" s="3">
         <v>0.29268499999999997</v>
       </c>
-      <c r="E112" s="7">
+      <c r="E112" s="3">
         <v>0.56237899999999996</v>
       </c>
-      <c r="F112" s="7"/>
-      <c r="G112" s="7"/>
-      <c r="H112" s="7"/>
+      <c r="F112" s="3"/>
+      <c r="G112" s="3"/>
+      <c r="H112" s="3"/>
     </row>
-    <row r="113" spans="3:8">
-      <c r="C113" s="7"/>
-      <c r="D113" s="7">
+    <row r="113" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C113" s="3"/>
+      <c r="D113" s="3">
         <v>0.31467299999999998</v>
       </c>
-      <c r="E113" s="7">
+      <c r="E113" s="3">
         <v>0.64422699999999999</v>
       </c>
-      <c r="F113" s="7"/>
-      <c r="G113" s="7"/>
-      <c r="H113" s="7"/>
+      <c r="F113" s="3"/>
+      <c r="G113" s="3"/>
+      <c r="H113" s="3"/>
     </row>
-    <row r="114" spans="3:8">
-      <c r="C114" s="7"/>
-      <c r="D114" s="7">
+    <row r="114" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C114" s="3"/>
+      <c r="D114" s="3">
         <v>0.33882800000000002</v>
       </c>
-      <c r="E114" s="7">
+      <c r="E114" s="3">
         <v>0.66002300000000003</v>
       </c>
-      <c r="F114" s="7"/>
-      <c r="G114" s="7"/>
-      <c r="H114" s="7"/>
+      <c r="F114" s="3"/>
+      <c r="G114" s="3"/>
+      <c r="H114" s="3"/>
     </row>
-    <row r="115" spans="3:8">
-      <c r="C115" s="7"/>
-      <c r="D115" s="7">
+    <row r="115" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C115" s="3"/>
+      <c r="D115" s="3">
         <v>0.369944</v>
       </c>
-      <c r="E115" s="7">
+      <c r="E115" s="3">
         <v>0.70802399999999999</v>
       </c>
-      <c r="F115" s="7"/>
-      <c r="G115" s="7"/>
-      <c r="H115" s="7"/>
+      <c r="F115" s="3"/>
+      <c r="G115" s="3"/>
+      <c r="H115" s="3"/>
     </row>
-    <row r="116" spans="3:8">
-      <c r="C116" s="7"/>
-      <c r="D116" s="7"/>
-      <c r="E116" s="7"/>
-      <c r="F116" s="7"/>
-      <c r="G116" s="7"/>
-      <c r="H116" s="7"/>
+    <row r="116" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C116" s="3"/>
+      <c r="D116" s="3"/>
+      <c r="E116" s="3"/>
+      <c r="F116" s="3"/>
+      <c r="G116" s="3"/>
+      <c r="H116" s="3"/>
     </row>
-    <row r="117" spans="3:8">
-      <c r="C117" s="7"/>
-      <c r="D117" s="7"/>
-      <c r="E117" s="7"/>
-      <c r="F117" s="7"/>
-      <c r="G117" s="7"/>
-      <c r="H117" s="7"/>
+    <row r="117" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C117" s="3"/>
+      <c r="D117" s="3"/>
+      <c r="E117" s="3"/>
+      <c r="F117" s="3"/>
+      <c r="G117" s="3"/>
+      <c r="H117" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -17754,12 +19214,12 @@
       <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
@@ -17770,7 +19230,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>0</v>
       </c>
@@ -17781,7 +19241,7 @@
         <v>8.3752999999999994E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -17792,7 +19252,7 @@
         <v>2.4433E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -17803,7 +19263,7 @@
         <v>1.2744999999999999E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -17814,7 +19274,7 @@
         <v>7.2610000000000001E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -17825,7 +19285,7 @@
         <v>5.0939999999999996E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -17836,7 +19296,7 @@
         <v>4.0990000000000002E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -17847,7 +19307,7 @@
         <v>3.0990000000000002E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>7</v>
       </c>
@@ -17857,15 +19317,15 @@
       <c r="C9" s="2">
         <v>2.5360000000000001E-3</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F9" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>8</v>
       </c>
@@ -17875,13 +19335,13 @@
       <c r="C10" s="2">
         <v>2.1700000000000001E-3</v>
       </c>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>9</v>
       </c>
@@ -17891,13 +19351,13 @@
       <c r="C11" s="2">
         <v>1.8829999999999999E-3</v>
       </c>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>10</v>
       </c>
@@ -17907,13 +19367,13 @@
       <c r="C12" s="2">
         <v>1.6559999999999999E-3</v>
       </c>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>11</v>
       </c>
@@ -17923,13 +19383,13 @@
       <c r="C13" s="2">
         <v>1.5499999999999999E-3</v>
       </c>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>12</v>
       </c>
@@ -17939,13 +19399,13 @@
       <c r="C14" s="2">
         <v>1.3810000000000001E-3</v>
       </c>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>13</v>
       </c>
@@ -17956,7 +19416,7 @@
         <v>1.2390000000000001E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>14</v>
       </c>
@@ -17967,7 +19427,7 @@
         <v>1.1460000000000001E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>15</v>
       </c>
@@ -17978,7 +19438,7 @@
         <v>1.0610000000000001E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>16</v>
       </c>
@@ -17989,7 +19449,7 @@
         <v>9.8900000000000008E-4</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>17</v>
       </c>
@@ -18000,7 +19460,7 @@
         <v>9.3800000000000003E-4</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>18</v>
       </c>
@@ -18011,7 +19471,7 @@
         <v>8.7299999999999997E-4</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>19</v>
       </c>
@@ -18022,7 +19482,7 @@
         <v>8.2600000000000002E-4</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>20</v>
       </c>

</xml_diff>